<commit_message>
add content MultiLinguals Seeder
</commit_message>
<xml_diff>
--- a/applications/FS.Abp.Demo/aspnet-core/src/FS.Abp.Demo.Domain.Shared/Files/Contents.xlsx
+++ b/applications/FS.Abp.Demo/aspnet-core/src/FS.Abp.Demo.Domain.Shared/Files/Contents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Further-PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\FS.Works0831\projects\FS.Abp\applications\FS.Abp.Demo\aspnet-core\src\FS.Abp.Demo.Domain.Shared\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4C67BB-BA6A-453A-9323-1EA4245DEDC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EBA0C4-1814-4E63-BA28-570602D2C74A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20700" yWindow="765" windowWidth="17280" windowHeight="11115" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blog" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="44">
   <si>
     <t>專任教師</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -177,26 +177,28 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>image</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>string</t>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>ImageUrl</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmailAddress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DateTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ImageUrl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -534,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -573,7 +575,7 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -587,7 +589,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -601,7 +603,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -613,6 +615,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="119" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -620,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE647956-37C1-4134-82CD-CD35A4A387AE}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -659,7 +662,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -673,7 +676,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -687,7 +690,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -701,7 +704,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -715,7 +718,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -729,7 +732,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -743,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -757,7 +760,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -771,7 +774,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -799,7 +802,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -824,7 +827,7 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -838,7 +841,7 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -852,7 +855,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -866,7 +869,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -905,7 +908,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -919,7 +922,7 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -933,7 +936,7 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -947,7 +950,7 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -961,7 +964,7 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -975,7 +978,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -989,7 +992,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -1028,7 +1031,7 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -1042,7 +1045,7 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -1056,7 +1059,7 @@
         <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -1084,7 +1087,7 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -1098,7 +1101,7 @@
         <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -1112,7 +1115,7 @@
         <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -1126,7 +1129,7 @@
         <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -1146,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA1A3F0-81B1-43E3-B0FB-7842C0770513}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1185,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1196,7 +1199,7 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1210,7 +1213,7 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1224,7 +1227,7 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1238,7 +1241,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1252,7 +1255,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C8">
         <v>1</v>

</xml_diff>